<commit_message>
V3.3 (output file done)
</commit_message>
<xml_diff>
--- a/Files/Assumptions_data.xlsx
+++ b/Files/Assumptions_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgouv\Desktop\IN+\Waste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgouv\PycharmProjects\IN+\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986C1792-2210-47E1-B383-45B5EB4F9B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1103F304-C9CC-42CC-BCDC-7DBF19B29B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{84341E79-AEA6-4457-B501-811FED569B63}"/>
   </bookViews>
@@ -131,10 +131,6 @@
     <t>Type of waste</t>
   </si>
   <si>
-    <t xml:space="preserve">Boreal and Temperate 
-(MAT ≤ 20°C) </t>
-  </si>
-  <si>
     <t>Tropical (MAT &gt; 20°C)</t>
   </si>
   <si>
@@ -381,9 +377,6 @@
     <t>Table 2.3: Correction factor for greenhouse gases (CO2eq)</t>
   </si>
   <si>
-    <t>Incineration facility efficiency (%)</t>
-  </si>
-  <si>
     <t>Type of incineration/technology</t>
   </si>
   <si>
@@ -448,6 +441,12 @@
   </si>
   <si>
     <t>Table 6.1: Anaerobic Digestion Parameters (SCW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boreal and Temperate (MAT ≤ 20°C) </t>
+  </si>
+  <si>
+    <t>Energy recovery efficiency (%)</t>
   </si>
 </sst>
 </file>
@@ -990,6 +989,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1121,12 +1126,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1464,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A24E25-EF29-4891-95C0-D378A933F9B2}">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:N105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,53 +1483,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="63"/>
     </row>
     <row r="2" spans="1:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="67" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66" t="s">
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66" t="s">
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="68"/>
-      <c r="N2" s="69"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1538,37 +1537,37 @@
         <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1585,7 +1584,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="1">
         <v>44</v>
@@ -1594,7 +1593,7 @@
         <v>40</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I4" s="1">
         <v>46</v>
@@ -1603,7 +1602,7 @@
         <v>42</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -1612,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1629,7 +1628,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1">
         <v>30</v>
@@ -1638,7 +1637,7 @@
         <v>25</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5" s="1">
         <v>50</v>
@@ -1647,7 +1646,7 @@
         <v>25</v>
       </c>
       <c r="K5" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L5" s="1">
         <v>20</v>
@@ -1656,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1682,7 +1681,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" s="1">
         <v>38</v>
@@ -1691,7 +1690,7 @@
         <v>20</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>18</v>
@@ -1717,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1">
         <v>50</v>
@@ -1726,7 +1725,7 @@
         <v>46</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="1">
         <v>50</v>
@@ -1735,7 +1734,7 @@
         <v>46</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>18</v>
@@ -1761,7 +1760,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1">
         <v>49</v>
@@ -1770,7 +1769,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="1">
         <v>49</v>
@@ -1779,7 +1778,7 @@
         <v>45</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L8" s="1">
         <v>0</v>
@@ -1805,7 +1804,7 @@
         <v>39</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1">
         <v>47</v>
@@ -1814,7 +1813,7 @@
         <v>47</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="1">
         <v>67</v>
@@ -1867,7 +1866,7 @@
         <v>67</v>
       </c>
       <c r="K10" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L10" s="1">
         <v>100</v>
@@ -1876,7 +1875,7 @@
         <v>95</v>
       </c>
       <c r="N10" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1999,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L13" s="13">
         <v>100</v>
@@ -2008,25 +2007,25 @@
         <v>50</v>
       </c>
       <c r="N13" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N14" s="29"/>
     </row>
     <row r="15" spans="1:14" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="D15" s="73" t="s">
+      <c r="B15" s="65"/>
+      <c r="D15" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="G15" s="70" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" s="72"/>
+      <c r="E15" s="76"/>
+      <c r="G15" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -2039,10 +2038,10 @@
         <v>24</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H16" s="47">
         <v>25</v>
@@ -2050,7 +2049,7 @@
     </row>
     <row r="17" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="37">
         <v>1</v>
@@ -2062,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H17" s="45">
         <v>298</v>
@@ -2070,7 +2069,7 @@
     </row>
     <row r="18" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="37">
         <v>0.5</v>
@@ -2084,7 +2083,7 @@
     </row>
     <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B19" s="37">
         <v>0.8</v>
@@ -2092,7 +2091,7 @@
     </row>
     <row r="20" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="38">
         <v>0.4</v>
@@ -2100,117 +2099,117 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="72"/>
+      <c r="A22" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="74"/>
     </row>
     <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="81" t="s">
+      <c r="I23" s="83"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="84"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="66"/>
+      <c r="B24" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="82"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
-      <c r="B24" s="67" t="s">
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67" t="s">
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67" t="s">
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" s="67"/>
-      <c r="M24" s="80"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="82"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="33">
         <v>17</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" s="33">
         <v>12</v>
@@ -2219,136 +2218,136 @@
         <v>22</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H26" s="33">
         <v>15</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J26" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K26" s="33">
         <v>10</v>
       </c>
       <c r="L26" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M26" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="33">
         <v>35</v>
       </c>
       <c r="C27" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="33" t="s">
         <v>73</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>74</v>
       </c>
       <c r="E27" s="33">
         <v>23</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H27" s="33">
         <v>28</v>
       </c>
       <c r="I27" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J27" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K27" s="33">
         <v>20</v>
       </c>
       <c r="L27" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M27" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="33">
         <v>14</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="33">
         <v>7</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H28" s="33">
         <v>11</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J28" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K28" s="33">
         <v>4</v>
       </c>
       <c r="L28" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M28" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="33">
         <v>12</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E29" s="33">
         <v>4</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H29" s="33">
         <v>8</v>
       </c>
       <c r="I29" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J29" s="33" t="s">
         <v>22</v>
@@ -2357,269 +2356,269 @@
         <v>2</v>
       </c>
       <c r="L29" s="33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M29" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="35">
         <v>14</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E30" s="35">
         <v>7</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H30" s="35">
         <v>11</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J30" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K30" s="35">
         <v>4</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M30" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="83" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="84"/>
-      <c r="C32" s="84"/>
-      <c r="D32" s="85"/>
-      <c r="F32" s="86" t="s">
-        <v>120</v>
-      </c>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="88"/>
-      <c r="K32" s="86" t="s">
-        <v>121</v>
-      </c>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="88"/>
+      <c r="A32" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
+      <c r="F32" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="90"/>
+      <c r="K32" s="88" t="s">
+        <v>119</v>
+      </c>
+      <c r="L32" s="89"/>
+      <c r="M32" s="89"/>
+      <c r="N32" s="90"/>
     </row>
     <row r="33" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>42</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="C33" s="17">
         <v>0.01</v>
       </c>
       <c r="D33" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" s="71"/>
+      <c r="K33" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="N33" s="71"/>
+    </row>
+    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="78"/>
+      <c r="B34" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="F33" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66" t="s">
-        <v>116</v>
-      </c>
-      <c r="I33" s="69"/>
-      <c r="K33" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="L33" s="66"/>
-      <c r="M33" s="66" t="s">
-        <v>122</v>
-      </c>
-      <c r="N33" s="69"/>
-    </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C34" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="89" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" s="90"/>
-      <c r="H34" s="90">
+        <v>43</v>
+      </c>
+      <c r="F34" s="91" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92">
         <v>0.2</v>
       </c>
-      <c r="I34" s="93"/>
-      <c r="K34" s="89" t="s">
-        <v>117</v>
-      </c>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90">
+      <c r="I34" s="95"/>
+      <c r="K34" s="91" t="s">
+        <v>115</v>
+      </c>
+      <c r="L34" s="92"/>
+      <c r="M34" s="92">
         <v>47</v>
       </c>
-      <c r="N34" s="93"/>
+      <c r="N34" s="95"/>
     </row>
     <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="76"/>
+      <c r="A35" s="78"/>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="6">
         <v>0.01</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="89" t="s">
-        <v>118</v>
-      </c>
-      <c r="G35" s="90"/>
-      <c r="H35" s="90">
+        <v>43</v>
+      </c>
+      <c r="F35" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="92"/>
+      <c r="H35" s="92">
         <v>6</v>
       </c>
-      <c r="I35" s="93"/>
-      <c r="K35" s="89" t="s">
-        <v>118</v>
-      </c>
-      <c r="L35" s="90"/>
-      <c r="M35" s="90">
+      <c r="I35" s="95"/>
+      <c r="K35" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="L35" s="92"/>
+      <c r="M35" s="92">
         <v>41</v>
       </c>
-      <c r="N35" s="93"/>
+      <c r="N35" s="95"/>
     </row>
     <row r="36" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="76"/>
+      <c r="A36" s="78"/>
       <c r="B36" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="6">
         <v>0.01</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="91" t="s">
-        <v>119</v>
-      </c>
-      <c r="G36" s="92"/>
-      <c r="H36" s="92">
+        <v>43</v>
+      </c>
+      <c r="F36" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="94"/>
+      <c r="H36" s="94">
         <v>60</v>
       </c>
-      <c r="I36" s="94"/>
-      <c r="K36" s="91" t="s">
-        <v>119</v>
-      </c>
-      <c r="L36" s="92"/>
-      <c r="M36" s="92">
+      <c r="I36" s="96"/>
+      <c r="K36" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="L36" s="94"/>
+      <c r="M36" s="94">
         <v>56</v>
       </c>
-      <c r="N36" s="94"/>
+      <c r="N36" s="96"/>
     </row>
     <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="76"/>
+      <c r="A37" s="78"/>
       <c r="B37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="77"/>
+      <c r="A38" s="79"/>
       <c r="B38" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C38" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="78" t="s">
+      <c r="A39" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="C39" s="6">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
+      <c r="A40" s="78"/>
       <c r="B40" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="79"/>
+      <c r="A41" s="81"/>
       <c r="B41" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="21">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" s="51"/>
-      <c r="D43" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="E43" s="51"/>
+      <c r="A43" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="53"/>
+      <c r="D43" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="53"/>
     </row>
     <row r="44" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="6">
         <v>0.5</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E44" s="6">
         <v>0.5</v>
@@ -2627,13 +2626,13 @@
     </row>
     <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="6">
         <v>0.01</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E45" s="6">
         <v>0.01</v>
@@ -2641,14 +2640,14 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="1">
         <f>44/12</f>
         <v>3.6666666666666665</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E46" s="1">
         <f>44/12</f>
@@ -2657,14 +2656,14 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B47" s="6">
         <f>16/12</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E47" s="6">
         <f>16/12</f>
@@ -2673,13 +2672,13 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
@@ -2687,37 +2686,37 @@
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="6">
         <v>0.5</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="B51" s="51"/>
-      <c r="D51" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="E51" s="51"/>
+      <c r="A51" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="53"/>
+      <c r="D51" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" s="53"/>
     </row>
     <row r="52" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="6">
         <v>0.5</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52" s="6">
         <v>0.5</v>
@@ -2725,13 +2724,13 @@
     </row>
     <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" s="6">
         <v>1</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="6">
         <v>1</v>
@@ -2739,14 +2738,14 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B54" s="1">
         <f>44/12</f>
         <v>3.6666666666666665</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E54" s="1">
         <f>44/12</f>
@@ -2755,14 +2754,14 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" s="6">
         <f>16/12</f>
         <v>1.3333333333333333</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="6">
         <f>16/12</f>
@@ -2771,13 +2770,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
@@ -2785,13 +2784,13 @@
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E57" s="1">
         <v>0.9</v>
@@ -2799,27 +2798,27 @@
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="6">
         <v>0.5</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E58" s="6">
         <v>0.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="51"/>
+      <c r="A60" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" s="53"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="B61" s="1">
         <v>21.2</v>
@@ -2827,7 +2826,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" s="1">
         <f>44/12</f>
@@ -2836,7 +2835,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -2844,7 +2843,7 @@
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B64" s="1">
         <v>60</v>
@@ -2852,21 +2851,21 @@
     </row>
     <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B65" s="1">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="B67" s="51"/>
+      <c r="A67" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="53"/>
     </row>
     <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B68" s="6">
         <v>0.5</v>
@@ -2874,7 +2873,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" s="6">
         <v>0.5</v>
@@ -2882,7 +2881,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B70" s="1">
         <f>44/12</f>
@@ -2891,7 +2890,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71" s="6">
         <f>16/12</f>
@@ -2900,7 +2899,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72" s="1">
         <v>0.1</v>
@@ -2908,7 +2907,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B73" s="1">
         <v>0.5</v>
@@ -2916,7 +2915,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B74" s="6">
         <v>0.5</v>
@@ -2924,7 +2923,7 @@
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B75" s="6">
         <v>0.5</v>
@@ -2932,7 +2931,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B76" s="6">
         <v>0.45</v>
@@ -2940,7 +2939,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B77" s="6">
         <f>44.01/16.04</f>
@@ -2948,48 +2947,48 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="B79" s="51"/>
+      <c r="A79" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" s="53"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="B82" s="51"/>
-      <c r="C82" s="51"/>
-      <c r="D82" s="51"/>
-      <c r="E82" s="51"/>
+      <c r="A82" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
+      <c r="E82" s="53"/>
     </row>
     <row r="83" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="43" t="s">
         <v>30</v>
       </c>
       <c r="B83" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C83" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C83" s="44" t="s">
-        <v>107</v>
-      </c>
       <c r="D83" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E83" s="44" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B84" s="1">
         <v>-1.5209999999999999</v>
@@ -3006,7 +3005,7 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B85" s="1">
         <v>-9.1080000000000005</v>
@@ -3023,7 +3022,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B86" s="1">
         <v>-0.53</v>
@@ -3040,7 +3039,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B87" s="1">
         <v>-1.8</v>
@@ -3074,7 +3073,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B89" s="1">
         <v>-0.63400000000000001</v>
@@ -3091,104 +3090,104 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B90" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C90" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D90" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E90" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B91" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B91" s="49" t="s">
-        <v>128</v>
-      </c>
       <c r="C91" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D91" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E91" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B92" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C92" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D92" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E92" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="B94" s="59"/>
-      <c r="C94" s="59"/>
-      <c r="D94" s="59"/>
-      <c r="E94" s="59"/>
-      <c r="F94" s="59"/>
-      <c r="G94" s="59"/>
-      <c r="H94" s="59"/>
-      <c r="I94" s="59"/>
-      <c r="J94" s="59"/>
-      <c r="K94" s="59"/>
-      <c r="L94" s="59"/>
-      <c r="M94" s="60"/>
-      <c r="N94" s="61"/>
+      <c r="A94" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B94" s="61"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
+      <c r="K94" s="61"/>
+      <c r="L94" s="61"/>
+      <c r="M94" s="62"/>
+      <c r="N94" s="63"/>
     </row>
     <row r="95" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="56" t="s">
-        <v>129</v>
+      <c r="A95" s="58" t="s">
+        <v>127</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C95" s="52" t="s">
+      <c r="C95" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="53"/>
-      <c r="E95" s="55"/>
-      <c r="F95" s="52" t="s">
+      <c r="D95" s="55"/>
+      <c r="E95" s="57"/>
+      <c r="F95" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="G95" s="53"/>
-      <c r="H95" s="55"/>
-      <c r="I95" s="52" t="s">
+      <c r="G95" s="55"/>
+      <c r="H95" s="57"/>
+      <c r="I95" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J95" s="53"/>
-      <c r="K95" s="55"/>
-      <c r="L95" s="52" t="s">
+      <c r="J95" s="55"/>
+      <c r="K95" s="57"/>
+      <c r="L95" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="M95" s="53"/>
-      <c r="N95" s="54"/>
+      <c r="M95" s="55"/>
+      <c r="N95" s="56"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="57"/>
+      <c r="A96" s="59"/>
       <c r="B96" s="3" t="s">
         <v>17</v>
       </c>
@@ -3196,42 +3195,42 @@
         <v>17</v>
       </c>
       <c r="D96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E96" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H96" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="I96" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K96" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="L96" s="3" t="s">
         <v>17</v>
       </c>
       <c r="M96" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N96" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="N96" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B97" s="41">
         <v>100</v>
@@ -3242,7 +3241,7 @@
       <c r="D97" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E97" s="95" t="s">
+      <c r="E97" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F97" s="2" t="s">
@@ -3251,31 +3250,31 @@
       <c r="G97" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H97" s="95" t="s">
+      <c r="H97" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I97" s="49" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="J97" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="K97" s="25" t="s">
-        <v>19</v>
+        <v>126</v>
+      </c>
+      <c r="K97" s="49" t="s">
+        <v>126</v>
       </c>
       <c r="L97" s="49" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="M97" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="N97" s="25" t="s">
-        <v>19</v>
+        <v>126</v>
+      </c>
+      <c r="N97" s="49" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B98" s="41">
         <v>100</v>
@@ -3286,7 +3285,7 @@
       <c r="D98" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E98" s="95" t="s">
+      <c r="E98" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F98" s="2" t="s">
@@ -3295,31 +3294,31 @@
       <c r="G98" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H98" s="95" t="s">
+      <c r="H98" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I98" s="49" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="J98" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="K98" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="L98" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="M98" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="N98" s="50" t="s">
-        <v>19</v>
+        <v>126</v>
+      </c>
+      <c r="K98" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="L98" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="M98" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="N98" s="49" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99" s="41">
         <v>100</v>
@@ -3330,7 +3329,7 @@
       <c r="D99" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E99" s="95" t="s">
+      <c r="E99" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F99" s="2" t="s">
@@ -3339,7 +3338,7 @@
       <c r="G99" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H99" s="95" t="s">
+      <c r="H99" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I99" s="49">
@@ -3349,21 +3348,21 @@
         <v>67</v>
       </c>
       <c r="K99" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="L99" s="96">
+        <v>69</v>
+      </c>
+      <c r="L99" s="52">
         <v>100</v>
       </c>
-      <c r="M99" s="96">
+      <c r="M99" s="52">
         <v>95</v>
       </c>
       <c r="N99" s="50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B100" s="41">
         <v>100</v>
@@ -3374,7 +3373,7 @@
       <c r="D100" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E100" s="95" t="s">
+      <c r="E100" s="51" t="s">
         <v>18</v>
       </c>
       <c r="F100" s="2" t="s">
@@ -3383,7 +3382,7 @@
       <c r="G100" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H100" s="95" t="s">
+      <c r="H100" s="51" t="s">
         <v>18</v>
       </c>
       <c r="I100" s="49">
@@ -3393,7 +3392,7 @@
         <v>67</v>
       </c>
       <c r="K100" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L100" s="49">
         <v>100</v>
@@ -3402,7 +3401,7 @@
         <v>95</v>
       </c>
       <c r="N100" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
@@ -3430,28 +3429,28 @@
       <c r="H101" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I101" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="J101" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="K101" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="L101" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="M101" s="96" t="s">
-        <v>19</v>
-      </c>
-      <c r="N101" s="96" t="s">
-        <v>19</v>
+      <c r="I101" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="J101" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="K101" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="L101" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="M101" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="N101" s="49" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102" s="41">
         <v>90</v>
@@ -3463,7 +3462,7 @@
         <v>36</v>
       </c>
       <c r="E102" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F102" s="1">
         <v>44</v>
@@ -3472,7 +3471,7 @@
         <v>40</v>
       </c>
       <c r="H102" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I102" s="49">
         <v>46</v>
@@ -3481,7 +3480,7 @@
         <v>42</v>
       </c>
       <c r="K102" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L102" s="49">
         <v>1</v>
@@ -3490,12 +3489,12 @@
         <v>0</v>
       </c>
       <c r="N102" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B103" s="1">
         <v>40</v>
@@ -3515,8 +3514,8 @@
       <c r="G103" s="1">
         <v>20</v>
       </c>
-      <c r="H103" s="1" t="s">
-        <v>66</v>
+      <c r="H103" s="49" t="s">
+        <v>65</v>
       </c>
       <c r="I103" s="1">
         <v>38</v>
@@ -3524,8 +3523,8 @@
       <c r="J103" s="1">
         <v>20</v>
       </c>
-      <c r="K103" s="1" t="s">
-        <v>66</v>
+      <c r="K103" s="49" t="s">
+        <v>65</v>
       </c>
       <c r="L103" s="48" t="s">
         <v>18</v>
@@ -3539,7 +3538,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B104" s="1">
         <v>85</v>
@@ -3551,7 +3550,7 @@
         <v>39</v>
       </c>
       <c r="E104" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F104" s="1">
         <v>50</v>
@@ -3559,8 +3558,8 @@
       <c r="G104" s="1">
         <v>46</v>
       </c>
-      <c r="H104" s="1" t="s">
-        <v>67</v>
+      <c r="H104" s="49" t="s">
+        <v>66</v>
       </c>
       <c r="I104" s="1">
         <v>50</v>
@@ -3568,8 +3567,8 @@
       <c r="J104" s="1">
         <v>46</v>
       </c>
-      <c r="K104" s="1" t="s">
-        <v>67</v>
+      <c r="K104" s="49" t="s">
+        <v>66</v>
       </c>
       <c r="L104" s="48" t="s">
         <v>18</v>
@@ -3583,7 +3582,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B105" s="1">
         <v>40</v>
@@ -3595,7 +3594,7 @@
         <v>18</v>
       </c>
       <c r="E105" s="49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F105" s="1">
         <v>49</v>
@@ -3603,8 +3602,8 @@
       <c r="G105" s="1">
         <v>45</v>
       </c>
-      <c r="H105" s="1" t="s">
-        <v>68</v>
+      <c r="H105" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="I105" s="1">
         <v>49</v>
@@ -3612,8 +3611,8 @@
       <c r="J105" s="1">
         <v>45</v>
       </c>
-      <c r="K105" s="1" t="s">
-        <v>68</v>
+      <c r="K105" s="49" t="s">
+        <v>67</v>
       </c>
       <c r="L105" s="1">
         <v>0</v>
@@ -3621,7 +3620,7 @@
       <c r="M105" s="1">
         <v>0</v>
       </c>
-      <c r="N105" s="1" t="s">
+      <c r="N105" s="49" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>